<commit_message>
Groundwater avail and stage of dev added
</commit_message>
<xml_diff>
--- a/PadaliHMS.xlsx
+++ b/PadaliHMS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rishabh\waterbudgeting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6C7EE9-30D1-47CF-B9AB-F3E62B69E2B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F81F0C-231F-40E4-BEF7-A5A8DDB2F2C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{72AEDC66-642F-4F7B-B82B-33FB806BBC45}"/>
   </bookViews>
@@ -445,7 +445,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>